<commit_message>
correcting twitter files upload problem
</commit_message>
<xml_diff>
--- a/uploads/media/Twitter_ID.xlsx
+++ b/uploads/media/Twitter_ID.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hi\django_project\uploads\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJAY\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,15 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>User name</t>
   </si>
   <si>
-    <t>@wkupin</t>
+    <t>@Ting2li</t>
   </si>
   <si>
-    <t>@Ting2li</t>
+    <t>@MB_Leonard</t>
+  </si>
+  <si>
+    <t>@wkupin</t>
   </si>
 </sst>
 </file>
@@ -121,12 +124,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -412,7 +418,7 @@
   <dimension ref="A1:A66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,12 +437,14 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>

</xml_diff>